<commit_message>
Changed models, added SHAP, changed scaler
</commit_message>
<xml_diff>
--- a/model-building/corr.xlsx
+++ b/model-building/corr.xlsx
@@ -457,27 +457,27 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9215913011934687</v>
+        <v>0.9215856593215532</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>x</t>
+          <t>y</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8844351610161171</v>
+        <v>0.8888175447215017</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>y</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8654208978641909</v>
+        <v>0.8872212110854774</v>
       </c>
     </row>
     <row r="6">
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8612494438514452</v>
+        <v>0.8821066056491267</v>
       </c>
     </row>
     <row r="7">
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1284202936903544</v>
+        <v>0.1282727869737869</v>
       </c>
     </row>
     <row r="8">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1271339021217227</v>
+        <v>0.1272413322081764</v>
       </c>
     </row>
     <row r="9">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.09712522851078023</v>
+        <v>0.09719151518199726</v>
       </c>
     </row>
     <row r="10">
@@ -527,7 +527,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0957059722000913</v>
+        <v>0.09525504563025693</v>
       </c>
     </row>
     <row r="11">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.08171035944819419</v>
+        <v>0.08188540924334869</v>
       </c>
     </row>
     <row r="12">
@@ -547,7 +547,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.05922286739196753</v>
+        <v>0.05873119343477257</v>
       </c>
     </row>
     <row r="13">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.01872822029558888</v>
+        <v>0.01876460707401062</v>
       </c>
     </row>
     <row r="14">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.008956633824945669</v>
+        <v>0.008963348666493816</v>
       </c>
     </row>
     <row r="15">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.008556125878215276</v>
+        <v>0.008511647393192818</v>
       </c>
     </row>
     <row r="16">
@@ -587,7 +587,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.006593487726256617</v>
+        <v>0.006862420000157086</v>
       </c>
     </row>
     <row r="17">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.0002553360644738753</v>
+        <v>-0.0001394779193105116</v>
       </c>
     </row>
     <row r="18">
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.0003120195356980056</v>
+        <v>-0.0003574708906823419</v>
       </c>
     </row>
     <row r="19">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.001061687930914593</v>
+        <v>-0.001094085972133455</v>
       </c>
     </row>
     <row r="20">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.009886258383741225</v>
+        <v>-0.009677735194627292</v>
       </c>
     </row>
     <row r="21">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.01064740458415539</v>
+        <v>-0.0106525476532575</v>
       </c>
     </row>
     <row r="22">
@@ -647,7 +647,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.02416086300318407</v>
+        <v>-0.02393224913792053</v>
       </c>
     </row>
     <row r="23">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0.04959600700348558</v>
+        <v>-0.04954682179790952</v>
       </c>
     </row>
     <row r="24">
@@ -667,7 +667,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-0.05238083127932953</v>
+        <v>-0.0522698070334784</v>
       </c>
     </row>
     <row r="25">
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.07247254410853911</v>
+        <v>-0.07252059251127617</v>
       </c>
     </row>
     <row r="26">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0.09526616537320358</v>
+        <v>-0.09544297924939737</v>
       </c>
     </row>
     <row r="27">
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-0.09717538486205374</v>
+        <v>-0.0969723330799748</v>
       </c>
     </row>
     <row r="28">
@@ -707,7 +707,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-0.1010893683312125</v>
+        <v>-0.1009108224223475</v>
       </c>
     </row>
     <row r="29">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-0.3068731789692042</v>
+        <v>-0.3070850070127243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>